<commit_message>
Updated coremark data after fixing bug in coremk_or0
</commit_message>
<xml_diff>
--- a/data/coremark-optimisations.xlsx
+++ b/data/coremark-optimisations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,8 +231,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -347,7 +349,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -401,6 +403,7 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -454,6 +457,7 @@
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -786,7 +790,7 @@
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="M43" sqref="A31:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -939,20 +943,20 @@
         <v>23</v>
       </c>
       <c r="E16">
-        <v>756.2</v>
+        <v>774.4</v>
       </c>
       <c r="F16">
         <f t="shared" ref="F16:F24" si="0">E16-H16-J16</f>
-        <v>115.40000000000003</v>
+        <v>124.29999999999995</v>
       </c>
       <c r="H16">
-        <v>360</v>
+        <v>361.3</v>
       </c>
       <c r="J16">
-        <v>280.8</v>
+        <v>288.8</v>
       </c>
       <c r="L16">
-        <v>756.7</v>
+        <v>775</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
@@ -963,20 +967,20 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>361.9</v>
+        <v>363.6</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>54.999999999999972</v>
+        <v>55.90000000000002</v>
       </c>
       <c r="H17">
-        <v>231.9</v>
+        <v>232</v>
       </c>
       <c r="J17">
-        <v>75</v>
+        <v>75.7</v>
       </c>
       <c r="L17">
-        <v>362.1</v>
+        <v>363.8</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1199,35 +1203,35 @@
       </c>
       <c r="F33" s="3">
         <f>F16</f>
-        <v>115.40000000000003</v>
+        <v>124.29999999999995</v>
       </c>
       <c r="G33" s="1">
         <f>(F33-F$32)/F$32</f>
-        <v>5.4469273743016808</v>
+        <v>5.9441340782122909</v>
       </c>
       <c r="H33" s="3">
         <f>H16</f>
-        <v>360</v>
+        <v>361.3</v>
       </c>
       <c r="I33" s="1">
         <f>(H33-H$32)/H$32</f>
-        <v>6.3170731707317076</v>
+        <v>6.3434959349593498</v>
       </c>
       <c r="J33" s="3">
         <f>J16</f>
-        <v>280.8</v>
+        <v>288.8</v>
       </c>
       <c r="K33" s="1">
         <f>(J33-J$32)/J$32</f>
-        <v>14.600000000000001</v>
+        <v>15.044444444444444</v>
       </c>
       <c r="L33" s="3">
         <f>L16</f>
-        <v>756.7</v>
+        <v>775</v>
       </c>
       <c r="M33" s="1">
         <f>(L33-L$32)/L$32</f>
-        <v>7.891891891891893</v>
+        <v>8.1069330199764984</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1239,35 +1243,35 @@
       </c>
       <c r="F34" s="3">
         <f>F17</f>
-        <v>54.999999999999972</v>
+        <v>55.90000000000002</v>
       </c>
       <c r="G34" s="1">
         <f>(F34-F$32)/F$32</f>
-        <v>2.0726256983240221</v>
+        <v>2.1229050279329633</v>
       </c>
       <c r="H34" s="3">
         <f>H17</f>
-        <v>231.9</v>
+        <v>232</v>
       </c>
       <c r="I34" s="1">
         <f>(H34-H$32)/H$32</f>
-        <v>3.713414634146341</v>
+        <v>3.7154471544715446</v>
       </c>
       <c r="J34" s="3">
         <f>J17</f>
-        <v>75</v>
+        <v>75.7</v>
       </c>
       <c r="K34" s="1">
         <f>(J34-J$32)/J$32</f>
-        <v>3.1666666666666665</v>
+        <v>3.2055555555555557</v>
       </c>
       <c r="L34" s="3">
         <f>L17</f>
-        <v>362.1</v>
+        <v>363.8</v>
       </c>
       <c r="M34" s="1">
         <f>(L34-L$32)/L$32</f>
-        <v>3.2549941245593423</v>
+        <v>3.2749706227967104</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -1279,35 +1283,35 @@
       </c>
       <c r="F35" s="3">
         <f>F18-F17</f>
-        <v>0.10000000000003695</v>
+        <v>-0.80000000000001137</v>
       </c>
       <c r="G35" s="1">
         <f>F35/F$32</f>
-        <v>5.5865921787730168E-3</v>
+        <v>-4.4692737430168251E-2</v>
       </c>
       <c r="H35" s="3">
         <f>H18-H17</f>
-        <v>-37.099999999999994</v>
+        <v>-37.199999999999989</v>
       </c>
       <c r="I35" s="1">
         <f>H35/H$32</f>
-        <v>-0.75406504065040636</v>
+        <v>-0.75609756097560943</v>
       </c>
       <c r="J35" s="3">
         <f>J18-J17</f>
-        <v>-16.799999999999997</v>
+        <v>-17.5</v>
       </c>
       <c r="K35" s="1">
         <f>J35/J$32</f>
-        <v>-0.93333333333333313</v>
+        <v>-0.97222222222222221</v>
       </c>
       <c r="L35" s="3">
         <f>L18-L17</f>
-        <v>-53.800000000000011</v>
+        <v>-55.5</v>
       </c>
       <c r="M35" s="1">
         <f>L35/L$32</f>
-        <v>-0.63219741480611058</v>
+        <v>-0.65217391304347827</v>
       </c>
     </row>
     <row r="36" spans="1:13">

</xml_diff>